<commit_message>
Updates to plotting and extraction scripts
</commit_message>
<xml_diff>
--- a/Nigeria/Research/urban_rural_transmission_analysis/manuscript_scripts/Potential_covariates.xlsx
+++ b/Nigeria/Research/urban_rural_transmission_analysis/manuscript_scripts/Potential_covariates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ifeomaozodiegwu/Box/NU-malaria-team/data/nigeria_dhs/data_analysis/src/Research/urban_rural_transmission_analysis/manuscript_scripts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Box\NU-malaria-team\data\nigeria_dhs\data_analysis\src\Research\urban_rural_transmission_analysis\manuscript_scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{251E4587-4B80-7544-B7F1-15218438A4EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18DD9A4D-C19B-4A6D-BCBE-BE799916FF68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28360" windowHeight="13420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="77">
   <si>
     <t xml:space="preserve">Potential  variables </t>
   </si>
@@ -78,9 +78,6 @@
     <t xml:space="preserve">Environmental variables </t>
   </si>
   <si>
-    <t xml:space="preserve">Precipitation </t>
-  </si>
-  <si>
     <t xml:space="preserve">DHS survey variables </t>
   </si>
   <si>
@@ -102,24 +99,12 @@
     <t xml:space="preserve">Distance to water bodies </t>
   </si>
   <si>
-    <t xml:space="preserve">Land surface temperature -day </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Land surface temperature -night </t>
-  </si>
-  <si>
     <t xml:space="preserve">Normalized difference vegetative index </t>
   </si>
   <si>
     <t xml:space="preserve">Population density (&lt;= 5 years) </t>
   </si>
   <si>
-    <t xml:space="preserve">Rainfall (historical) </t>
-  </si>
-  <si>
-    <t>Rainfall (current)</t>
-  </si>
-  <si>
     <t>Entomological variables ??</t>
   </si>
   <si>
@@ -147,9 +132,6 @@
     <t xml:space="preserve">source </t>
   </si>
   <si>
-    <t>https://datacatalog.worldbank.org/dataset/world-terrain-elevation-above-sea-level-ele-gis-data-global-solar-atlas</t>
-  </si>
-  <si>
     <t>https://wopr.worldpop.org/?NGA/Buildings/v1.1</t>
   </si>
   <si>
@@ -159,23 +141,138 @@
     <t>using facebook data for all (https://data.humdata.org/organization/facebook?q=nigeria&amp;ext_page_size=25)</t>
   </si>
   <si>
-    <t>https://e4ftl01.cr.usgs.gov/MOLT/MOD11C3.006/</t>
-  </si>
-  <si>
-    <t>https://gpm.nasa.gov/data/directory</t>
-  </si>
-  <si>
-    <t>MAP</t>
-  </si>
-  <si>
-    <t>https://malariaatlas.org/data-project/covariates/</t>
+    <t xml:space="preserve">definition </t>
+  </si>
+  <si>
+    <t>Temperature of air at 2m above the surface of land, sea or in-land waters. 2m temperature is calculated by interpolating between the lowest model level and the Earth's surface, taking account of the atmospheric conditions. Temperature measured in kelvin can be converted to degrees Celsius (°C) by subtracting 273.15.</t>
+  </si>
+  <si>
+    <t>https://cds.climate.copernicus.eu/cdsapp#!/dataset/reanalysis-era5-land-monthly-means?tab=overview</t>
+  </si>
+  <si>
+    <t>Accumulated liquid and frozen water, including rain and snow, that falls to the Earth's surface. It is the sum of large-scale precipitation (that precipitation which is generated by large-scale weather patterns, such as troughs and cold fronts) and convective precipitation (generated by convection which occurs when air at lower levels in the atmosphere is warmer and less dense than the air above, so it rises). Precipitation variables do not include fog, dew or the precipitation that evaporates in the atmosphere before it lands at the surface of the Earth. This variable is accumulated from the beginning of the forecast time to the end of the forecast step. The units of precipitation are depth in metres. It is the depth the water would have if it were spread evenly over the grid box. Care should be taken when comparing model variables with observations, because observations are often local to a particular point in space and time, rather than representing averages over a model grid box and model time step.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Air temperature monthly </t>
+  </si>
+  <si>
+    <t>Air temperature monthly mean across alll years up till survey year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total monthly precipitation (current) </t>
+  </si>
+  <si>
+    <t>Total monthly precipitation averaged across all years up till survey year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://data.humdata.org/dataset/nigeria-water-courses; </t>
+  </si>
+  <si>
+    <t>https://datacatalog.worldbank.org/dataset/world-terrain-elevation-above-sea-level-ele-gis-data-global-solar-atlas; 
+https://globalsolaratlas.info/</t>
+  </si>
+  <si>
+    <t>Dominant malaria vector species globally, 2010</t>
+  </si>
+  <si>
+    <t>This layer shows the set of mosquito species that have been assessed as the most important for malaria transmission in each malaria endemic area. We used the predictive maps for each species to generate this multiple vector species map and only those areas with a presence probability greater than 0.5 were included. Our Technical Advisory Group (TAG) identified the three most important vector species per country (where there were three or more species) and ranked these species by their relative importance and the top-ranked species were displayed preferentially. In those areas where the dominance of one species was not clear, the predictive maps for each dominant species were merged. For Africa, the layer illustrates the distribution of those species considered to be of major importance. There are other important vector species so a second map of Africa dedicated to showing the distributions of these 'secondary' dominant vector species is also provided.</t>
+  </si>
+  <si>
+    <t>Secondary dominant malaria vector species in Africa+, 2010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accessibility variables </t>
+  </si>
+  <si>
+    <t>https://malariaatlas.org/trends/country/NGA</t>
+  </si>
+  <si>
+    <t>This friction surface quantifies the time required to traverse each pixel within an approximately one-by one-kilometer gridded representation of the Earth’s surface. The movement rates encapsulated within the friction surfaces were based on landscape characteristics and transportation infrastructure, and no individual movement data was used to create them. The friction surfaces were made by combining geographic datasets that each characterize a layer-specific cost of moving through the landscape. These datasets consisted of roads, railways, navigable waterways, bodies of water, land cover types, topographic conditions (elevation and slope angle), and national borders. Descriptions of these datasets and their associated processing steps are provided in Weiss et al. (2018). Note, however, that we did not consider air travel in this analysis.
+The road layers used to derive the friction surfaces were the most critical inputs for overall model accuracy. The roads datasets used for this project were the OSM and Google Roads datasets. OSM roads data were extracted in October 2019 and converted into a rasterized surface of road types whereby the fastest road type in each pixel took precedence. In a second processing step, the OSM data were analyzed to determine the median speed limit value for each road type in each country (extended data 1). These values were subsequently used to attribute road speeds to specific pixels using a lookup table. In cases where a road type was present in a country, but associated speed limit information was unavailable, a global average speed limit for that road type was used instead. The Google roads data consisted of a distance to road layer, which effectively became a rasterized roads surface by defining all pixels with distance values of less than 500 meters as roads. Because the OSM data were split by road type for which we had speed limit information, these roads data took precedence when both datasets indicated the existence of roads within a pixel. In cases where only Google roads data indicated the presence of a road, those pixels were assigned the generic “road” classification for purposes of assigning speed limits via the lookup tables. While the approach for making the friction surface was identical to the one used in Weiss et al. (2018), reanalysis was warranted because substantial additions have since been made to OSM. These changes included the addition of many previously missing roads, particularly in developing countries; and far more comprehensive speed limit information to support country-specific road speed attribution.</t>
+  </si>
+  <si>
+    <t>Global friction surface enumerating land-based travel speed with access to motorized transport for a nominal year 2019; minutes required to travel one metre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Global travel time to healthcare map with access to motorized transport; estimated travel time (minutes) to nearest healthcare facility
+</t>
+  </si>
+  <si>
+    <t>This is a map showing the estimated time to travel from every point on earth to the nearest healthcare facility by motorized transport. Travel times were calculated to the nearest geolocated hospital or clinic. A critical assumption of the travel time calculations, however, was that people moved through the landscape at an optimal speed. In the optimal friction surface, we assumed that humans traveling along roadways, railways, and on water moved at the motorized movement rates assigned to each type.
+We utilized healthcare facility locations from two of the largest global databases: (1) OpenStreetMap (OSM) data that was collated and made available for download at www.healthsites.io29; and (2) data from Google Maps that was extracted specifically for this project. We augmented the global datasets with continental-scale facility locations that were recently published for Africa (Maina, J. et al., 2019) and Australia (Barbieri, S. &amp; Jorm, 2019). To align temporally, each of these datasets was extracted in mid-2019. To facilitate comparisons between data sources, we used only facilities defined as hospitals and clinics, which matched the definition used in Maina, J. et al. (2019) and Barbieri, S. &amp; Jorm (2019), and was distinguishable within the OSM data by using the facility-type attribute. In contrast, Google Maps data were filtered to isolate hospitals and clinics from the full set of geolocated entities. For each dataset, multiple points found within the same approximately one-by-one-kilometer pixel were merged to match the resolution of the subsequent travel time maps.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Global friction surface enumerating land-based travel walking-only speed without access to motorized transport for a nominal year 2019;
+minutes required to travel one metre
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This friction surface quantifies the time required to traverse each pixel within an approximately one-by one-kilometer gridded representation of the Earth’s surface. The movement rates encapsulated within the friction surfaces were based on landscape characteristics and transportation infrastructure, and no individual movement data was used to create them. The friction surfaces were made by combining geographic datasets that each characterize a layer-specific cost of moving through the landscape. These datasets consisted of roads, railways, navigable waterways, bodies of water, land cover types, topographic conditions (elevation and slope angle), and national borders. Descriptions of these datasets and their associated processing steps are provided in Weiss et al. (2018). Note, however, that we did not consider air travel in this analysis.
+In this walking-only friction surface, we assumed that all road travel was limited to a walking speed of five kilometers per hour and all water travel was reduced to the rate for traversing a wetland or swimming of 1.0 kilometer per hour. The walking-only friction provided an upper bound of movement rates for individuals who lack access to, or cannot use, motorized transport.
+</t>
+  </si>
+  <si>
+    <t>Walking-only travel time to healthcare map without access to motorized transport; estimated travel time (minutes) to nearest healthcare facility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is a map showing the estimated time to travel from every point on earth to the nearest healthcare facility by walking. Travel times were calculated to the nearest geolocated hospital or clinic. A critical assumption of the travel time calculations, however, was that people moved through the landscape at an optimal speed. In the walking-only friction surface, we assumed that all road travel was limited to a walking speed of five kilometers per hour and all water travel was reduced to the rate for traversing a wetland or swimming of 1.0 kilometer per hour.
+We utilized healthcare facility locations from two of the largest global databases: (1) OpenStreetMap (OSM) data that was collated and made available for download at www.healthsites.io29; and (2) data from Google Maps that was extracted specifically for this project. We augmented the global datasets with continental-scale facility locations that were recently published for Africa (Maina, J. et al., 2019) and Australia (Barbieri, S. &amp; Jorm, 2019). To align temporally, each of these datasets was extracted in mid-2019. To facilitate comparisons between data sources, we used only facilities defined as hospitals and clinics, which matched the definition used in Maina, J. et al. (2019) and Barbieri, S. &amp; Jorm (2019), and was distinguishable within the OSM data by using the facility-type attribute. In contrast, Google Maps data were filtered to isolate hospitals and clinics from the full set of geolocated entities. For each dataset, multiple points found within the same approximately one-by-one-kilometer pixel were merged to match the resolution of the subsequent travel time maps.
+</t>
+  </si>
+  <si>
+    <t>A global map of travel time to cities to assess inequalities in accessibility in 2015; predicted travel time (minutes) to nearest city</t>
+  </si>
+  <si>
+    <t>This is a predictive map showing the estimated time to travel from every point on earth to the nearest (in time) city.</t>
+  </si>
+  <si>
+    <t>A global friction surface enumerating land-based travel speed for a nominal year 2015; minutes required to travel one metre</t>
+  </si>
+  <si>
+    <t>This global friction surface enumerates land-based travel speed for all land pixels between 85 degrees north and 60 degrees south for a nominal year 2015. This map was produced through a collaboration between MAP (University of Oxford), Google, the European Union Joint Research Centre (JRC), and the University of Twente, Netherlands. The underlying datasets used to produce the map include roads (comprising the first ever global-scale use of Open Street Map and Google roads datasets), railways, rivers, lakes, oceans, topographic conditions (slope and elevation), landcover types, and national borders. These datasets were each allocated a speed or speeds of travel in terms of time to cross each pixel of that type. The datasets were then combined to produce this "friction surface"; a map where every pixel is allocated a nominal overall speed of travel based on the types occurring within that pixel, with the fastest travel mode intersecting the pixel being used to determine the speed of travel in that pixel (with some exceptions such as national boundaries, which have the effect of imposing a travel time penalty). This map represents the travel speed from this allocation process, expressed in units of minutes required to travel one metre. It forms the underlying dataset behind the global accessibility map described in the referenced paper.</t>
+  </si>
+  <si>
+    <t>Prevalence of improved housing in sub-saharan africa, in 2000</t>
+  </si>
+  <si>
+    <t>This predictive surface shows the prevalence of improved housing in 2000, predicted at 5 x 5-km2 resolution. For further details see https://map.ox.ac.uk/research-project/housing_in_africa/</t>
+  </si>
+  <si>
+    <t>Prevalence of improved housing in sub-saharan africa, in 2015</t>
+  </si>
+  <si>
+    <t>This predictive surface shows the prevalence of improved housing in 2015, predicted at 5 x 5-km2 resolution. For further details see https://map.ox.ac.uk/research-project/housing_in_africa/</t>
+  </si>
+  <si>
+    <t>DHS</t>
+  </si>
+  <si>
+    <t>responsible person</t>
+  </si>
+  <si>
+    <t>Chilo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ifeoma </t>
+  </si>
+  <si>
+    <t>Chilo (will check if there is better dataset)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chilo </t>
+  </si>
+  <si>
+    <t>https://sedac.ciesin.columbia.edu/data/set/gpw-v4-population-count-adjusted-to-2015-unwpp-country-totals-rev11</t>
+  </si>
+  <si>
+    <t>The Gridded Population of the World, Version 4 (GPWv4): Population Count Adjusted to Match 2015 Revision of UN WPP Country Totals, Revision 11 consists of estimates of human population (number of persons per pixel) consistent with national censuses and population registers with respect to relative spatial distribution, but adjusted to match the 2015 Revision of the United Nation's World Population Prospects (UN WPP) country totals for the years 2000, 2005, 2010, 2015, and 2020. A proportional allocation gridding algorithm, utilizing approximately 13.5 million national and sub-national administrative units, was used to assign population counts to 30 arc-second grid cells. The data files were produced as global rasters at 30 arc-second (~1 km at the equator) resolution. To enable faster global processing, and in support of research communities, the 30 arc-second adjusted count data were aggregated to 2.5 arc-minute, 15 arc-minute, 30 arc-minute and 1 degree resolutions.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -187,6 +284,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -215,15 +320,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -502,332 +618,588 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52.5" customWidth="1"/>
-    <col min="2" max="2" width="37.33203125" customWidth="1"/>
+    <col min="1" max="1" width="61.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="110.5703125" customWidth="1"/>
+    <col min="5" max="5" width="134.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" t="s">
         <v>38</v>
       </c>
-      <c r="C1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
         <v>35</v>
       </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>7</v>
       </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="B16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>8</v>
       </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="B17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>9</v>
       </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+      <c r="B18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+      <c r="B19" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="B18" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>37</v>
       </c>
       <c r="B20" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>14</v>
       </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="B25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>15</v>
       </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+      <c r="B26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>17</v>
-      </c>
-      <c r="B27">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29">
         <v>0</v>
       </c>
-      <c r="C27" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="C29" t="s">
+        <v>72</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>73</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" s="3">
+        <v>1</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" s="3">
+        <v>1</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>24</v>
-      </c>
-      <c r="B28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>42</v>
-      </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
-      <c r="C29" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>25</v>
-      </c>
-      <c r="B30">
-        <v>0</v>
-      </c>
-      <c r="C30" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>27</v>
-      </c>
-      <c r="B32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>29</v>
       </c>
       <c r="B33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C33" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D34" t="s">
+        <v>40</v>
+      </c>
+      <c r="E34" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E35" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>48</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38" t="s">
+        <v>71</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E38" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>50</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39" t="s">
+        <v>71</v>
+      </c>
+      <c r="D39" t="s">
+        <v>52</v>
+      </c>
+      <c r="E39" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
+      <c r="B42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>36</v>
-      </c>
-      <c r="B40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+      <c r="B43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>19</v>
       </c>
-      <c r="B41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+      <c r="B44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>20</v>
       </c>
-      <c r="B42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
+      <c r="B47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>21</v>
-      </c>
-      <c r="B45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>23</v>
-      </c>
-      <c r="B46">
+      <c r="B48">
         <v>0</v>
       </c>
     </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>54</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51" t="s">
+        <v>71</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52" t="s">
+        <v>71</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E52" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53" t="s">
+        <v>71</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E53" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54" t="s">
+        <v>71</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E54" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="C55" t="s">
+        <v>71</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E55" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="C56" t="s">
+        <v>71</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E56" t="s">
+        <v>64</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D29" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D30" r:id="rId2" display="https://datacatalog.worldbank.org/dataset/world-terrain-elevation-above-sea-level-ele-gis-data-global-solar-atlas" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D38" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="D51" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="D52" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="D53" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="D54" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="D55" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="D56" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="D13" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="D35" r:id="rId11" location="!/dataset/reanalysis-era5-land-monthly-means?tab=overview" xr:uid="{6D7169C1-19A7-44F7-B09C-B6E8260104CF}"/>
+    <hyperlink ref="D9" r:id="rId12" xr:uid="{97DEA96F-BFCC-4080-A440-F24B10C07604}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>